<commit_message>
not id col supported enum
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/测试.xlsx
+++ b/src/test/resources/excel/测试.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>ID</t>
   </si>
@@ -28,6 +28,9 @@
     <t>活动时间段</t>
   </si>
   <si>
+    <t>道具ID</t>
+  </si>
+  <si>
     <t>100ms</t>
   </si>
   <si>
@@ -37,6 +40,9 @@
     <t>[2022-10-01,2022-10-08]</t>
   </si>
   <si>
+    <t>Item1</t>
+  </si>
+  <si>
     <t>1s</t>
   </si>
   <si>
@@ -50,6 +56,9 @@
   </si>
   <si>
     <t>12h</t>
+  </si>
+  <si>
+    <t>Item2</t>
   </si>
   <si>
     <t>14d</t>
@@ -63,12 +72,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,6 +94,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF9876AA"/>
+      <name val="Menlo"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -92,23 +108,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -116,7 +154,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -138,92 +176,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,13 +254,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,169 +416,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,22 +466,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -481,6 +492,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -515,17 +535,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,152 +550,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -691,6 +707,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1011,23 +1030,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="11.6428571428571" customWidth="1"/>
     <col min="3" max="3" width="23.5089285714286" style="2" customWidth="1"/>
     <col min="4" max="4" width="29.7589285714286" customWidth="1"/>
+    <col min="5" max="5" width="8.28571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:4">
+    <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1040,74 +1060,95 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
must check err msg
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/测试.xlsx
+++ b/src/test/resources/excel/测试.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11660" tabRatio="826"/>
+    <workbookView windowWidth="28800" windowHeight="11060" tabRatio="826"/>
   </bookViews>
   <sheets>
     <sheet name="礼包" sheetId="2" r:id="rId1"/>
@@ -70,9 +70,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -99,20 +99,42 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -122,14 +144,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -143,6 +189,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -151,92 +234,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,67 +257,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,109 +401,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,8 +448,17 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -473,6 +482,32 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -493,26 +528,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -527,168 +542,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1032,7 +1032,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="6" outlineLevelCol="5"/>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>5</v>
+        <v>2001</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>6</v>
+        <v>2002</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>

</xml_diff>